<commit_message>
DB uniqueness checker added
</commit_message>
<xml_diff>
--- a/usernames.xlsx
+++ b/usernames.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>usernames</t>
   </si>
@@ -34,7 +34,7 @@
     <t>Abcfinance*20</t>
   </si>
   <si>
-    <t>2020-03-01 17:28:53.787276</t>
+    <t>2020-03-07 00:13:44.591811</t>
   </si>
   <si>
     <t>100160423W</t>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t>100160619W</t>
-  </si>
-  <si>
-    <t>2020-03-01 17:29:02.416060</t>
   </si>
 </sst>
 </file>
@@ -424,10 +421,10 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4">

</xml_diff>

<commit_message>
reload 3 times when error
</commit_message>
<xml_diff>
--- a/usernames.xlsx
+++ b/usernames.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>usernames</t>
   </si>
@@ -34,7 +34,7 @@
     <t>Abcfinance*20</t>
   </si>
   <si>
-    <t>2020-03-07 00:13:44.591811</t>
+    <t>2020-03-13 00:18:39.043948</t>
   </si>
   <si>
     <t>100160423W</t>
@@ -43,7 +43,7 @@
     <t>Idfjobs*0505</t>
   </si>
   <si>
-    <t>2020-03-01 15:38:54.922127</t>
+    <t>2020-03-13 01:59:22.479527</t>
   </si>
   <si>
     <t>100160403W</t>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>100160619W</t>
+  </si>
+  <si>
+    <t>2020-03-13 02:08:39.637561</t>
   </si>
 </sst>
 </file>
@@ -421,7 +424,7 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>200</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -435,7 +438,7 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>80</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -449,10 +452,10 @@
         <v>11</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4">

</xml_diff>